<commit_message>
Update Budget Tracking Dashboard.xlsx
</commit_message>
<xml_diff>
--- a/Budget Tracking Dashboard.xlsx
+++ b/Budget Tracking Dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Analytics Projects\Data-Analyst-Project\Data-Analyst-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8C9A0F1-3172-4BFA-B3BB-44EE256B0AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66318324-EC0A-45C2-89F4-0297EF44999B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10656" yWindow="492" windowWidth="12384" windowHeight="11868" activeTab="1" xr2:uid="{870CEF35-62BB-45A3-98FE-45452197DEF6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{870CEF35-62BB-45A3-98FE-45452197DEF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$4:$A$9</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$4:$B$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$4:$A$9</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$4:$B$9</definedName>
     <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$A$11:$A$16</definedName>
     <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$B$11:$B$16</definedName>
   </definedNames>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Budget Tracking Dashboard</t>
   </si>
@@ -104,7 +106,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +144,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="ADLaM Display"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,7 +188,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -194,6 +201,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -234,11 +244,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -248,11 +258,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Percentage</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Breakdown of Budget</a:t>
+              <a:t>Percentage Breakdown of Budget</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -267,8 +273,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18921529775955248"/>
-          <c:y val="0.125"/>
+          <c:x val="0.18192135173475307"/>
+          <c:y val="1.8960616731953733E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -284,11 +290,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -307,10 +313,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30511745406824148"/>
-          <c:y val="0.29966717701953921"/>
-          <c:w val="0.3790382764654418"/>
-          <c:h val="0.63173046077573636"/>
+          <c:x val="0.24959495803765272"/>
+          <c:y val="0.29056173254725065"/>
+          <c:w val="0.50918851192983583"/>
+          <c:h val="0.62177290652738748"/>
         </c:manualLayout>
       </c:layout>
       <c:doughnutChart>
@@ -328,13 +334,17 @@
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="20000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -352,13 +362,17 @@
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="20000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -367,31 +381,80 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{018F8C8E-95D1-4872-B3D3-E4983B874964}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-827C-406F-A231-98E985FCFCA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{31769377-52C1-4FC6-8211-63469B921D34}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-AU"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-827C-406F-A231-98E985FCFCA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:pattFill prst="pct75">
-                <a:fgClr>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:sysClr>
-                </a:fgClr>
-                <a:bgClr>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:bgClr>
-              </a:pattFill>
+              <a:noFill/>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -400,7 +463,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -416,18 +479,19 @@
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
-                <a:ln w="9525">
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
                     </a:schemeClr>
                   </a:solidFill>
+                  <a:round/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -492,15 +556,20 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31277070304483545"/>
+          <c:y val="0.20632328308207706"/>
+          <c:w val="0.3744585939103291"/>
+          <c:h val="7.0666323744707799E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -513,9 +582,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -539,30 +608,14 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -592,10 +645,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1869,144 +1922,87 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -2018,19 +2014,22 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -2040,19 +2039,17 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -2062,14 +2059,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -2082,14 +2077,17 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -2100,7 +2098,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2116,19 +2114,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2138,22 +2138,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2162,17 +2163,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2181,12 +2182,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -2200,36 +2201,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -2239,28 +2234,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2269,35 +2253,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2306,35 +2291,27 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2342,22 +2319,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2365,14 +2331,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2384,12 +2350,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2398,13 +2364,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2413,9 +2380,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2425,19 +2392,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2446,16 +2414,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2463,8 +2426,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2473,16 +2442,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2518,8 +2487,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="609600" y="548640"/>
-              <a:ext cx="3566160" cy="2720340"/>
+              <a:off x="502920" y="1463040"/>
+              <a:ext cx="4495800" cy="3086100"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2552,15 +2521,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
@@ -2596,8 +2565,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4876800" y="548640"/>
-              <a:ext cx="4008120" cy="2758440"/>
+              <a:off x="5425440" y="1432560"/>
+              <a:ext cx="4008120" cy="3040380"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2630,15 +2599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3149,14 +3118,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE5BC5A-B720-49FF-9B6B-A03DF2680D94}">
-  <dimension ref="A1"/>
+  <dimension ref="I2:P3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+    </row>
+    <row r="3" spans="9:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I2:P3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>